<commit_message>
small changes / optimizations before implementing wages
</commit_message>
<xml_diff>
--- a/MISC/work hours database.xlsx
+++ b/MISC/work hours database.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Android\WorkRecordsPro\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Android\WorkRecordsPro\MISC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10836" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7332" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>EndDate</t>
+  </si>
+  <si>
+    <t>Notes!</t>
   </si>
 </sst>
 </file>
@@ -537,10 +540,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -621,128 +624,134 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="H5" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="7" t="s">
+    <row r="11" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D11" s="2" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D12" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+    <row r="15" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="7" t="s">
+    <row r="16" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="B16" s="7" t="s">
+    <row r="17" spans="2:2" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="7" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new jobs with (new) Pay Rates, save shift and calculate wages
</commit_message>
<xml_diff>
--- a/MISC/work hours database.xlsx
+++ b/MISC/work hours database.xlsx
@@ -12,7 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7332" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Database Tables" sheetId="1" r:id="rId1"/>
+    <sheet name="Features" sheetId="2" r:id="rId2"/>
+    <sheet name="Preferencess files" sheetId="4" r:id="rId3"/>
+    <sheet name="Shifts attributes" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -77,18 +80,12 @@
     <t>If job-pay date &gt; shift start and &lt; shift end, pay has been updated during the shift</t>
   </si>
   <si>
-    <t>OVERTIME</t>
-  </si>
-  <si>
     <t>PROCENT?</t>
   </si>
   <si>
     <t>OVERTIME_JOB</t>
   </si>
   <si>
-    <t>OvertimeID</t>
-  </si>
-  <si>
     <t>Overtime_meta?</t>
   </si>
   <si>
@@ -135,6 +132,51 @@
   </si>
   <si>
     <t>Notes!</t>
+  </si>
+  <si>
+    <t>New Shift</t>
+  </si>
+  <si>
+    <t>Quick Shift</t>
+  </si>
+  <si>
+    <t>Copy Shift ?</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Break(unpaid)</t>
+  </si>
+  <si>
+    <t>Total Paid</t>
+  </si>
+  <si>
+    <t>ok?</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Preferences</t>
+  </si>
+  <si>
+    <t>24H</t>
+  </si>
+  <si>
+    <t>overtime</t>
+  </si>
+  <si>
+    <t>overtime 2</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Tips</t>
   </si>
 </sst>
 </file>
@@ -543,7 +585,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -569,13 +611,13 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -585,14 +627,14 @@
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>0</v>
+      <c r="D2" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -602,11 +644,11 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>18</v>
+      <c r="D3" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>5</v>
@@ -614,24 +656,30 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -641,8 +689,8 @@
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>19</v>
+      <c r="D7" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -652,63 +700,55 @@
       <c r="B8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>20</v>
+      <c r="D8" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>4</v>
+      <c r="D9" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="H10" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="D11" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="H11" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D12" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="H13" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -718,11 +758,8 @@
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>4</v>
-      </c>
       <c r="H14" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -732,22 +769,16 @@
       <c r="B15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="H15" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="H16" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="46.8" x14ac:dyDescent="0.3">
@@ -759,4 +790,119 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>